<commit_message>
Ready to merge with DNPlanning. Data and specially costs are not realistic
</commit_message>
<xml_diff>
--- a/DG_param.xlsx
+++ b/DG_param.xlsx
@@ -363,20 +363,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -404,24 +404,192 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0.02</v>
+      </c>
+      <c r="C2">
+        <v>0.8</v>
+      </c>
+      <c r="D2">
+        <v>300000</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>7.35</v>
+      </c>
+      <c r="G2">
+        <v>1.5</v>
+      </c>
+      <c r="H2">
+        <v>0.3</v>
+      </c>
+      <c r="I2">
+        <v>0.3</v>
+      </c>
       <c r="J2">
-        <v>0.125</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>0.02</v>
+      </c>
+      <c r="C3">
+        <v>0.8</v>
+      </c>
+      <c r="D3">
+        <v>300000</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>7.35</v>
+      </c>
+      <c r="G3">
+        <v>1.5</v>
+      </c>
+      <c r="H3">
+        <v>0.3</v>
+      </c>
+      <c r="I3">
+        <v>0.3</v>
+      </c>
       <c r="J3">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0.02</v>
+      </c>
+      <c r="C4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D4">
+        <v>600000</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>45</v>
+      </c>
+      <c r="G4">
+        <v>8.5</v>
+      </c>
+      <c r="H4">
+        <v>0.45</v>
+      </c>
+      <c r="I4">
+        <v>0.45</v>
+      </c>
       <c r="J4">
-        <v>1.1880999999999999</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="C5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5">
+        <v>600000</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <v>8.5</v>
+      </c>
+      <c r="H5">
+        <v>0.45</v>
+      </c>
+      <c r="I5">
+        <v>0.45</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.02</v>
+      </c>
+      <c r="C6">
+        <v>1.5</v>
+      </c>
+      <c r="D6">
+        <v>900000</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>95</v>
+      </c>
+      <c r="G6">
+        <v>15.3</v>
+      </c>
+      <c r="H6">
+        <v>0.9</v>
+      </c>
+      <c r="I6">
+        <v>0.9</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.02</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>900000</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>95</v>
+      </c>
+      <c r="G7">
+        <v>15.3</v>
+      </c>
+      <c r="H7">
+        <v>0.9</v>
+      </c>
+      <c r="I7">
+        <v>0.9</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>